<commit_message>
added well test content model
added well test content model
</commit_message>
<xml_diff>
--- a/Links/ObjectClass-Property/ObjectClass-Property.xlsx
+++ b/Links/ObjectClass-Property/ObjectClass-Property.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Links\ObjectClass-Property\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\MIXITE\Projects\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Links\ObjectClass-Property\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t>def/property/feature-identifier</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>ObjectClass Label</t>
+  </si>
+  <si>
+    <t>def/object-class/well-test-observation</t>
   </si>
 </sst>
 </file>
@@ -575,21 +578,6 @@
           </cell>
           <cell r="B53" t="str">
             <v>Well Test Observation</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -2683,10 +2671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A10" sqref="A10:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2845,6 +2833,70 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="str">
+        <f>LOOKUP(B10,[1]ObjectClass!$A:$A,[1]ObjectClass!$B:$B)</f>
+        <v>Well Test Observation</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>LOOKUP(D10,[2]Property!$A:$A,[2]Property!$B:$B)</f>
+        <v>Feature Identifier</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="str">
+        <f>LOOKUP(B11,[1]ObjectClass!$A:$A,[1]ObjectClass!$B:$B)</f>
+        <v>Well Test Observation</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>LOOKUP(D11,[2]Property!$A:$A,[2]Property!$B:$B)</f>
+        <v>Feature Name</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="str">
+        <f>LOOKUP(B12,[1]ObjectClass!$A:$A,[1]ObjectClass!$B:$B)</f>
+        <v>Well Test Observation</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>LOOKUP(D12,[2]Property!$A:$A,[2]Property!$B:$B)</f>
+        <v>Feature Type</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="str">
+        <f>LOOKUP(B13,[1]ObjectClass!$A:$A,[1]ObjectClass!$B:$B)</f>
+        <v>Well Test Observation</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>LOOKUP(D13,[2]Property!$A:$A,[2]Property!$B:$B)</f>
+        <v>Location</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>